<commit_message>
file uploaded successfully in separate collections
</commit_message>
<xml_diff>
--- a/server/files/Employeedetails.xlsx
+++ b/server/files/Employeedetails.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathi\PAYSLIP\server\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47B7A2D-FC64-41AA-A65D-DADA4ABCC964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employeedetails" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -282,8 +288,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -883,7 +889,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -915,9 +921,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -949,6 +973,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1124,32 +1166,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11.33203125" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1">
+    <row r="1" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1202,7 +1244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1256,7 +1298,7 @@
         <v>805206087</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1310,7 +1352,7 @@
         <v>805206087</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1364,7 +1406,7 @@
         <v>805206087</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1418,7 +1460,7 @@
         <v>805206087</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1472,7 +1514,7 @@
         <v>805206087</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1526,7 +1568,7 @@
         <v>805206087</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1580,7 +1622,7 @@
         <v>805206087</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1634,7 +1676,7 @@
         <v>805206087</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1684,7 +1726,7 @@
         <v>555301000000000</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1734,7 +1776,7 @@
         <v>399502000000</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1784,7 +1826,7 @@
         <v>6031348562</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1834,7 +1876,7 @@
         <v>399502000000</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1884,7 +1926,7 @@
         <v>189801000000</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1934,7 +1976,7 @@
         <v>32347886858</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1984,7 +2026,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -2034,7 +2076,7 @@
         <v>38487137291</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2084,7 +2126,7 @@
         <v>3261100000000</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -2134,7 +2176,7 @@
         <v>18691100000000</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -2184,7 +2226,7 @@
         <v>500101000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -2234,7 +2276,7 @@
         <v>612937528</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -2284,7 +2326,7 @@
         <v>50100100000000</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -2334,7 +2376,7 @@
         <v>149201000000000</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -2384,7 +2426,7 @@
         <v>6245416712</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -2434,7 +2476,7 @@
         <v>2648100000000</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -2480,7 +2522,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2526,7 +2568,7 @@
         <v>913010000000000</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -2572,7 +2614,7 @@
         <v>32468506686</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -2618,7 +2660,7 @@
         <v>341002000000000</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -2664,7 +2706,7 @@
         <v>32098190001</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -2708,7 +2750,7 @@
         <v>10073647368</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -2754,7 +2796,7 @@
         <v>500101000000000</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2798,7 +2840,7 @@
         <v>71891900000000</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Lop and Salary logic Completed
</commit_message>
<xml_diff>
--- a/server/files/Employeedetails.xlsx
+++ b/server/files/Employeedetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathi\PAYSLIP\server\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47B7A2D-FC64-41AA-A65D-DADA4ABCC964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9234A0C5-D2A9-4AD8-9724-068859D35E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="85">
   <si>
     <t>Salary</t>
   </si>
@@ -283,6 +281,12 @@
   </si>
   <si>
     <t>Other_allowance</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>January</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1174,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,7 +1285,9 @@
       <c r="K2" s="1">
         <v>0</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="1">
+        <v>4</v>
+      </c>
       <c r="M2" s="1" t="s">
         <v>75</v>
       </c>
@@ -1335,7 +1341,9 @@
       <c r="K3" s="1">
         <v>0</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1">
+        <v>2</v>
+      </c>
       <c r="M3" s="1" t="s">
         <v>70</v>
       </c>
@@ -1389,7 +1397,9 @@
       <c r="K4" s="1">
         <v>0</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
       <c r="M4" s="1" t="s">
         <v>71</v>
       </c>
@@ -1443,7 +1453,9 @@
       <c r="K5" s="1">
         <v>0</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
       <c r="M5" s="1" t="s">
         <v>72</v>
       </c>
@@ -1497,7 +1509,9 @@
       <c r="K6" s="1">
         <v>0</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
       <c r="M6" s="1" t="s">
         <v>73</v>
       </c>
@@ -1551,7 +1565,9 @@
       <c r="K7" s="1">
         <v>0</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
       <c r="M7" s="1" t="s">
         <v>74</v>
       </c>
@@ -1605,7 +1621,9 @@
       <c r="K8" s="1">
         <v>0</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
       <c r="M8" s="1" t="s">
         <v>70</v>
       </c>
@@ -1659,7 +1677,9 @@
       <c r="K9" s="1">
         <v>0</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
       <c r="M9" s="1" t="s">
         <v>70</v>
       </c>
@@ -1713,9 +1733,15 @@
       <c r="K10" s="1">
         <v>0</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="L10" s="1">
+        <v>3</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2019</v>
+      </c>
       <c r="O10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1763,9 +1789,15 @@
       <c r="K11" s="1">
         <v>0</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="L11" s="1">
+        <v>5</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N11" s="1">
+        <v>2020</v>
+      </c>
       <c r="O11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1813,9 +1845,15 @@
       <c r="K12" s="1">
         <v>0</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="L12" s="1">
+        <v>3</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12" s="1">
+        <v>2019</v>
+      </c>
       <c r="O12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1863,9 +1901,15 @@
       <c r="K13" s="1">
         <v>0</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="L13" s="1">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" s="1">
+        <v>2020</v>
+      </c>
       <c r="O13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1913,9 +1957,15 @@
       <c r="K14" s="1">
         <v>0</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="L14" s="1">
+        <v>3</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" s="1">
+        <v>2018</v>
+      </c>
       <c r="O14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1963,9 +2013,15 @@
       <c r="K15" s="1">
         <v>0</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="L15" s="1">
+        <v>3</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2021</v>
+      </c>
       <c r="O15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2013,9 +2069,15 @@
       <c r="K16" s="1">
         <v>0</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="L16" s="1">
+        <v>3</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16" s="1">
+        <v>2020</v>
+      </c>
       <c r="O16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2063,9 +2125,15 @@
       <c r="K17" s="1">
         <v>0</v>
       </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="L17" s="1">
+        <v>3</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N17" s="1">
+        <v>2018</v>
+      </c>
       <c r="O17" s="1" t="s">
         <v>16</v>
       </c>
@@ -2113,9 +2181,15 @@
       <c r="K18" s="1">
         <v>0</v>
       </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="L18" s="1">
+        <v>3</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N18" s="1">
+        <v>2019</v>
+      </c>
       <c r="O18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2163,9 +2237,15 @@
       <c r="K19" s="1">
         <v>0</v>
       </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+      <c r="L19" s="1">
+        <v>3</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2020</v>
+      </c>
       <c r="O19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2213,9 +2293,15 @@
       <c r="K20" s="1">
         <v>0</v>
       </c>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="L20" s="1">
+        <v>3</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N20" s="1">
+        <v>2021</v>
+      </c>
       <c r="O20" s="1" t="s">
         <v>20</v>
       </c>
@@ -2263,9 +2349,15 @@
       <c r="K21" s="1">
         <v>0</v>
       </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="L21" s="1">
+        <v>3</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2021</v>
+      </c>
       <c r="O21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2313,9 +2405,15 @@
       <c r="K22" s="1">
         <v>0</v>
       </c>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="L22" s="1">
+        <v>3</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N22" s="1">
+        <v>2021</v>
+      </c>
       <c r="O22" s="1" t="s">
         <v>16</v>
       </c>
@@ -2363,9 +2461,15 @@
       <c r="K23" s="1">
         <v>0</v>
       </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="L23" s="1">
+        <v>3</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N23" s="1">
+        <v>2021</v>
+      </c>
       <c r="O23" s="1" t="s">
         <v>20</v>
       </c>
@@ -2413,9 +2517,15 @@
       <c r="K24" s="1">
         <v>0</v>
       </c>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
+      <c r="L24" s="1">
+        <v>3</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N24" s="1">
+        <v>2021</v>
+      </c>
       <c r="O24" s="1" t="s">
         <v>20</v>
       </c>
@@ -2463,9 +2573,15 @@
       <c r="K25" s="1">
         <v>0</v>
       </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="L25" s="1">
+        <v>3</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2021</v>
+      </c>
       <c r="O25" s="1" t="s">
         <v>20</v>
       </c>
@@ -2511,9 +2627,15 @@
       <c r="K26" s="1">
         <v>0</v>
       </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
+      <c r="L26" s="1">
+        <v>3</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N26" s="1">
+        <v>2021</v>
+      </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1" t="s">
         <v>47</v>
@@ -2557,9 +2679,15 @@
       <c r="K27" s="1">
         <v>0</v>
       </c>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
+      <c r="L27" s="1">
+        <v>3</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N27" s="1">
+        <v>2021</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1" t="s">
         <v>49</v>
@@ -2603,9 +2731,15 @@
       <c r="K28" s="1">
         <v>0</v>
       </c>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
+      <c r="L28" s="1">
+        <v>3</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N28" s="1">
+        <v>2023</v>
+      </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1" t="s">
         <v>51</v>
@@ -2649,9 +2783,15 @@
       <c r="K29" s="1">
         <v>0</v>
       </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
+      <c r="L29" s="1">
+        <v>3</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N29" s="1">
+        <v>2023</v>
+      </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1" t="s">
         <v>53</v>
@@ -2695,9 +2835,15 @@
       <c r="K30" s="1">
         <v>0</v>
       </c>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
+      <c r="L30" s="1">
+        <v>3</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N30" s="1">
+        <v>2023</v>
+      </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1" t="s">
         <v>55</v>
@@ -2741,9 +2887,15 @@
       <c r="K31" s="1">
         <v>0</v>
       </c>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
+      <c r="L31" s="1">
+        <v>3</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N31" s="1">
+        <v>2023</v>
+      </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1">
@@ -2785,9 +2937,15 @@
       <c r="K32" s="1">
         <v>0</v>
       </c>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
+      <c r="L32" s="1">
+        <v>3</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N32" s="1">
+        <v>2023</v>
+      </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1" t="s">
         <v>58</v>
@@ -2829,9 +2987,15 @@
       <c r="K33" s="1">
         <v>0</v>
       </c>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
+      <c r="L33" s="1">
+        <v>3</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N33" s="1">
+        <v>2023</v>
+      </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1" t="s">
         <v>60</v>
@@ -2867,9 +3031,15 @@
       <c r="K34" s="1">
         <v>0</v>
       </c>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
+      <c r="L34" s="1">
+        <v>3</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N34" s="1">
+        <v>2023</v>
+      </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>

</xml_diff>